<commit_message>
update gitignore, add test data
</commit_message>
<xml_diff>
--- a/testdata/lists/Beschreibung_de.xlsx
+++ b/testdata/lists/Beschreibung_de.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/lists/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A82E6-B086-B94B-ACBF-84C85828F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>Schichteigenschaften</t>
   </si>
@@ -77,28 +86,27 @@
   </si>
   <si>
     <t>Gruppiert</t>
+  </si>
+  <si>
+    <t>zweite Unterliste</t>
+  </si>
+  <si>
+    <t>dritte Unterliste</t>
+  </si>
+  <si>
+    <t>Knoten der zweiten Unterliste</t>
+  </si>
+  <si>
+    <t>Spezialzeichen 1&amp;2-%*_0 sind eingebettet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -108,21 +116,15 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -130,50 +132,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -184,24 +165,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,7 +445,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -422,7 +464,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -452,7 +494,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -478,7 +520,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -504,7 +546,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -530,7 +572,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -556,7 +598,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -582,7 +624,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -608,7 +650,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -634,7 +676,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -660,7 +702,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -673,9 +715,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -692,7 +740,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -711,7 +759,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -737,7 +785,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -763,7 +811,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +837,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -815,7 +863,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -841,7 +889,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -867,7 +915,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -893,7 +941,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -919,7 +967,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +993,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -958,9 +1006,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -974,7 +1028,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -993,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1023,7 +1077,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1049,7 +1103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,7 +1129,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1101,7 +1155,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1181,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1153,7 +1207,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1233,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1259,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1231,7 +1285,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,392 +1298,430 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="4" width="22.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" customWidth="1"/>
-    <col min="8" max="8" width="66" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24" style="6" customWidth="1"/>
+    <col min="2" max="4" width="22.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19" style="6" customWidth="1"/>
+    <col min="8" max="8" width="66" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s" s="5">
+    <row r="1" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s" s="5">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s" s="5">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="5">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s" s="5">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="5">
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s" s="5">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s" s="5">
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s" s="5">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="5">
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s" s="5">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s" s="5">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s" s="5">
+      <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s" s="5">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s" s="5">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s" s="5">
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s" s="5">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s" s="5">
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" ht="17" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s" s="5">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="s" s="5">
+      <c r="C11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s" s="5">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s" s="5">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" t="s" s="5">
+      <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s" s="5">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s" s="5">
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s" s="5">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="s" s="5">
+      <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" ht="17" customHeight="1">
-      <c r="A15" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s" s="5">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" ht="17" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s" s="5">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s" s="5">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s" s="5">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s" s="5">
+      <c r="C17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s" s="5">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s" s="5">
+      <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" ht="17" customHeight="1">
-      <c r="A19" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s" s="5">
+      <c r="D18" s="4"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s" s="5">
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" ht="17" customHeight="1">
-      <c r="A20" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s" s="5">
+      <c r="D19" s="4"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s" s="5">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" ht="17" customHeight="1">
-      <c r="A21" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s" s="5">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" t="s" s="5">
+      <c r="C21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s" s="5">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s" s="7">
+      <c r="C22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
update german test file
</commit_message>
<xml_diff>
--- a/testdata/lists/Beschreibung_de.xlsx
+++ b/testdata/lists/Beschreibung_de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A82E6-B086-B94B-ACBF-84C85828F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BA4AF0-35DB-5641-B8C5-53A72B092610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5840" yWindow="1060" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>Schichteigenschaften</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Spezialzeichen 1&amp;2-%*_0 sind eingebettet</t>
+  </si>
+  <si>
+    <t>sehr</t>
+  </si>
+  <si>
+    <t>tief</t>
+  </si>
+  <si>
+    <t>verschachtelt!</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1719,6 +1728,48 @@
         <v>25</v>
       </c>
     </row>
+    <row r="27" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
corrected test data, added some error messages
</commit_message>
<xml_diff>
--- a/testdata/lists/Beschreibung_de.xlsx
+++ b/testdata/lists/Beschreibung_de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BA4AF0-35DB-5641-B8C5-53A72B092610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D233F548-0CB7-2F4F-8027-46A8B3314E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="1060" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-16300" windowWidth="26880" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,73 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
-  <si>
-    <t>Schichteigenschaften</t>
-  </si>
-  <si>
-    <t>Textur (Körnung)</t>
-  </si>
-  <si>
-    <t>Ton</t>
-  </si>
-  <si>
-    <t>Silt</t>
-  </si>
-  <si>
-    <t>Sand</t>
-  </si>
-  <si>
-    <t>Feinsand</t>
-  </si>
-  <si>
-    <t>Mittelsand</t>
-  </si>
-  <si>
-    <t>Grobsand</t>
-  </si>
-  <si>
-    <t>Kies</t>
-  </si>
-  <si>
-    <t>Feinkies</t>
-  </si>
-  <si>
-    <t>Mittelkies</t>
-  </si>
-  <si>
-    <t>Grobkies</t>
-  </si>
-  <si>
-    <t>Gerölle</t>
-  </si>
-  <si>
-    <t>Blöcke</t>
-  </si>
-  <si>
-    <t>Schichtung</t>
-  </si>
-  <si>
-    <t>Geschichtet</t>
-  </si>
-  <si>
-    <t>Laminiert</t>
-  </si>
-  <si>
-    <t>fining upward</t>
-  </si>
-  <si>
-    <t>coarsening upward</t>
-  </si>
-  <si>
-    <t>Horizontale Einregelung</t>
-  </si>
-  <si>
-    <t>Ungeschichtet</t>
-  </si>
-  <si>
-    <t>Gruppiert</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
   <si>
     <t>zweite Unterliste</t>
   </si>
@@ -100,13 +34,58 @@
     <t>Spezialzeichen 1&amp;2-%*_0 sind eingebettet</t>
   </si>
   <si>
-    <t>sehr</t>
-  </si>
-  <si>
     <t>tief</t>
   </si>
   <si>
     <t>verschachtelt!</t>
+  </si>
+  <si>
+    <t>erste Unterliste</t>
+  </si>
+  <si>
+    <t>erster Listenknoten</t>
+  </si>
+  <si>
+    <t>zweiter Listenknoten</t>
+  </si>
+  <si>
+    <t>eins</t>
+  </si>
+  <si>
+    <t>zwei</t>
+  </si>
+  <si>
+    <t>drei</t>
+  </si>
+  <si>
+    <t>vier</t>
+  </si>
+  <si>
+    <t>fünf</t>
+  </si>
+  <si>
+    <t>sechs</t>
+  </si>
+  <si>
+    <t>sieben</t>
+  </si>
+  <si>
+    <t>fein</t>
+  </si>
+  <si>
+    <t>mittel</t>
+  </si>
+  <si>
+    <t>grob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sehr          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">             sehr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sehr  </t>
   </si>
 </sst>
 </file>
@@ -1328,14 +1307,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="117" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="4" width="22.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.83203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="6" customWidth="1"/>
     <col min="7" max="7" width="19" style="6" customWidth="1"/>
@@ -1346,7 +1326,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1358,10 +1338,10 @@
     </row>
     <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1372,13 +1352,13 @@
     </row>
     <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1388,13 +1368,13 @@
     </row>
     <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1404,13 +1384,13 @@
     </row>
     <row r="5" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1420,16 +1400,16 @@
     </row>
     <row r="6" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1438,16 +1418,16 @@
     </row>
     <row r="7" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1456,16 +1436,16 @@
     </row>
     <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1474,13 +1454,13 @@
     </row>
     <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1490,16 +1470,16 @@
     </row>
     <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1508,16 +1488,16 @@
     </row>
     <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1526,16 +1506,16 @@
     </row>
     <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1544,13 +1524,13 @@
     </row>
     <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1560,13 +1540,13 @@
     </row>
     <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1576,10 +1556,10 @@
     </row>
     <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1590,13 +1570,13 @@
     </row>
     <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1606,13 +1586,13 @@
     </row>
     <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1622,13 +1602,13 @@
     </row>
     <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="8"/>
@@ -1638,13 +1618,13 @@
     </row>
     <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="8"/>
@@ -1654,13 +1634,13 @@
     </row>
     <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1670,13 +1650,13 @@
     </row>
     <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1686,13 +1666,13 @@
     </row>
     <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1702,72 +1682,72 @@
     </row>
     <row r="23" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test: add unittest for excel to json lists (DEV-534) (#157)
* update gitignore, add test data

* first draft

* finished unit test

* update german test file

* add jsonpath_ng to requirements.txt

* add pandas to requirements.txt

* correct bazel

* corrected test data, added some error messages

* corrected test data

* import jsonpath_ng.ext separately

* improvement: take the english label instead of the node name, because the node name can differ because of its appended counter

* implement reviewer's feedback
</commit_message>
<xml_diff>
--- a/testdata/lists/Beschreibung_de.xlsx
+++ b/testdata/lists/Beschreibung_de.xlsx
@@ -1,104 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/lists/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6568D06-590B-0C4A-B36B-DCE3F1BEBB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="-16300" windowWidth="26880" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
-  <si>
-    <t>Schichteigenschaften</t>
-  </si>
-  <si>
-    <t>Textur (Körnung)</t>
-  </si>
-  <si>
-    <t>Ton</t>
-  </si>
-  <si>
-    <t>Silt</t>
-  </si>
-  <si>
-    <t>Sand</t>
-  </si>
-  <si>
-    <t>Feinsand</t>
-  </si>
-  <si>
-    <t>Mittelsand</t>
-  </si>
-  <si>
-    <t>Grobsand</t>
-  </si>
-  <si>
-    <t>Kies</t>
-  </si>
-  <si>
-    <t>Feinkies</t>
-  </si>
-  <si>
-    <t>Mittelkies</t>
-  </si>
-  <si>
-    <t>Grobkies</t>
-  </si>
-  <si>
-    <t>Gerölle</t>
-  </si>
-  <si>
-    <t>Blöcke</t>
-  </si>
-  <si>
-    <t>Schichtung</t>
-  </si>
-  <si>
-    <t>Geschichtet</t>
-  </si>
-  <si>
-    <t>Laminiert</t>
-  </si>
-  <si>
-    <t>fining upward</t>
-  </si>
-  <si>
-    <t>coarsening upward</t>
-  </si>
-  <si>
-    <t>Horizontale Einregelung</t>
-  </si>
-  <si>
-    <t>Ungeschichtet</t>
-  </si>
-  <si>
-    <t>Gruppiert</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
+  <si>
+    <t>zweite Unterliste</t>
+  </si>
+  <si>
+    <t>dritte Unterliste</t>
+  </si>
+  <si>
+    <t>Knoten der zweiten Unterliste</t>
+  </si>
+  <si>
+    <t>Spezialzeichen 1&amp;2-%*_0 sind eingebettet</t>
+  </si>
+  <si>
+    <t>tief</t>
+  </si>
+  <si>
+    <t>verschachtelt!</t>
+  </si>
+  <si>
+    <t>erste Unterliste</t>
+  </si>
+  <si>
+    <t>erster Listenknoten</t>
+  </si>
+  <si>
+    <t>zweiter Listenknoten</t>
+  </si>
+  <si>
+    <t>eins</t>
+  </si>
+  <si>
+    <t>zwei</t>
+  </si>
+  <si>
+    <t>drei</t>
+  </si>
+  <si>
+    <t>vier</t>
+  </si>
+  <si>
+    <t>fünf</t>
+  </si>
+  <si>
+    <t>sechs</t>
+  </si>
+  <si>
+    <t>sieben</t>
+  </si>
+  <si>
+    <t>fein</t>
+  </si>
+  <si>
+    <t>mittel</t>
+  </si>
+  <si>
+    <t>grob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sehr          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">             sehr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sehr  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -108,21 +104,15 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -130,50 +120,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -184,24 +153,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,7 +433,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -422,7 +452,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -452,7 +482,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -478,7 +508,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -504,7 +534,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -530,7 +560,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -556,7 +586,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -582,7 +612,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -608,7 +638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -634,7 +664,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -660,7 +690,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -673,9 +703,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -692,7 +728,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -711,7 +747,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -737,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -763,7 +799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +825,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -815,7 +851,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -841,7 +877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -867,7 +903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -893,7 +929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -919,7 +955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -958,9 +994,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -974,7 +1016,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -993,7 +1035,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1023,7 +1065,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1049,7 +1091,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,7 +1117,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1101,7 +1143,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1127,7 +1169,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1153,7 +1195,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1179,7 +1221,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1205,7 +1247,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1231,7 +1273,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,392 +1286,473 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:E29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="4" width="22.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" customWidth="1"/>
-    <col min="8" max="8" width="66" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.83203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19" style="6" customWidth="1"/>
+    <col min="8" max="8" width="66" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s" s="5">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s" s="5">
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="5">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s" s="5">
+      <c r="C27" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="5">
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s" s="5">
+    </row>
+    <row r="29" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s" s="5">
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s" s="5">
+      <c r="E29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" ht="17" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="5">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" ht="17" customHeight="1">
-      <c r="A15" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" ht="17" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" ht="17" customHeight="1">
-      <c r="A19" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" ht="17" customHeight="1">
-      <c r="A20" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" ht="17" customHeight="1">
-      <c r="A21" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740200000000005" bottom="0.78740200000000005" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>